<commit_message>
Added config stub and dynamic highlighting
</commit_message>
<xml_diff>
--- a/tests/202205/First_Company-202205.xlsx
+++ b/tests/202205/First_Company-202205.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\CodeHagen\GitHub\TMetric2Excel\tests\202205\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FWHagen\TMetric2Excel\tests\202205\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3989E50-5199-4DA6-9110-676E91BAD14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6A66AC1-C30A-4206-98AB-DD7A5A4BA23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3000" yWindow="1335" windowWidth="24060" windowHeight="13590" xr2:uid="{324FEB65-5CD5-4424-8F76-4481F45EC839}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11325" xr2:uid="{0E381D9F-39CC-4B8F-A346-5C5084460295}"/>
   </bookViews>
   <sheets>
     <sheet name="202205" sheetId="1" r:id="rId1"/>
@@ -483,7 +483,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C5BBABD-9A4C-46E2-9413-79F62E97C97E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215436B8-76A2-4D8E-A61C-4FEFF798D998}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1269,6 +1269,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added support for Rounding to Whole Hour and bugfixes to config parsing
</commit_message>
<xml_diff>
--- a/tests/202205/First_Company-202205.xlsx
+++ b/tests/202205/First_Company-202205.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FWHagen\TMetric2Excel\tests\202205\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6A66AC1-C30A-4206-98AB-DD7A5A4BA23F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{06523BD8-3F30-4088-A571-72C2E9679ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11325" xr2:uid="{0E381D9F-39CC-4B8F-A346-5C5084460295}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11265" xr2:uid="{B2361929-F983-486A-8A0D-FA4A27AB8C27}"/>
   </bookViews>
   <sheets>
     <sheet name="202205" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -483,7 +484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{215436B8-76A2-4D8E-A61C-4FEFF798D998}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D807FA71-B268-4A0F-A168-9626EA424665}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Refactored test writers, moved summaries under col 1 with indentions, and added widths to headers
</commit_message>
<xml_diff>
--- a/tests/202205/First_Company-202205.xlsx
+++ b/tests/202205/First_Company-202205.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\FWHagen\TMetric2Excel\tests\202205\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06523BD8-3F30-4088-A571-72C2E9679ABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{686782F9-1784-486C-A5A1-0E20A5C48507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11265" xr2:uid="{B2361929-F983-486A-8A0D-FA4A27AB8C27}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11265" xr2:uid="{FCA70FFC-E766-49AD-9ECE-C14E332AFDD4}"/>
   </bookViews>
   <sheets>
     <sheet name="202205" sheetId="1" r:id="rId1"/>
@@ -159,18 +159,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,15 +494,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D807FA71-B268-4A0F-A168-9626EA424665}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E0889C8-644D-43C0-B527-A34C668A678E}">
   <dimension ref="A1:F53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="9.140625" style="4"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="5" width="16.7109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -511,7 +522,7 @@
       <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="11" t="s">
         <v>16</v>
       </c>
     </row>
@@ -540,19 +551,19 @@
       <c r="A3" s="2">
         <v>44683</v>
       </c>
-      <c r="B3" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="3">
         <v>6</v>
       </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3">
         <v>1.5</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <f>SUM(B3:E3)</f>
         <v>8</v>
       </c>
@@ -561,19 +572,19 @@
       <c r="A4" s="2">
         <v>44684</v>
       </c>
-      <c r="B4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C4" s="4">
+      <c r="B4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C4" s="3">
         <v>5</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <v>1.5</v>
       </c>
-      <c r="E4" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F4" s="4">
+      <c r="E4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F4" s="3">
         <f>SUM(B4:E4)</f>
         <v>7.5</v>
       </c>
@@ -582,19 +593,19 @@
       <c r="A5" s="2">
         <v>44685</v>
       </c>
-      <c r="B5" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
+      <c r="B5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
         <v>7.5</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <f>SUM(B5:E5)</f>
         <v>9</v>
       </c>
@@ -603,19 +614,19 @@
       <c r="A6" s="2">
         <v>44686</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="4">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
         <v>1.5</v>
       </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
         <f>SUM(B6:E6)</f>
         <v>6.5</v>
       </c>
@@ -624,19 +635,19 @@
       <c r="A7" s="2">
         <v>44687</v>
       </c>
-      <c r="B7" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
+      <c r="B7" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C7" s="3">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3">
         <v>2</v>
       </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
         <f>SUM(B7:E7)</f>
         <v>2.5</v>
       </c>
@@ -687,19 +698,19 @@
       <c r="A10" s="2">
         <v>44690</v>
       </c>
-      <c r="B10" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C10" s="4">
-        <v>0</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="B10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3">
         <v>6.5</v>
       </c>
-      <c r="E10" s="4">
-        <v>0</v>
-      </c>
-      <c r="F10" s="4">
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
         <f>SUM(B10:E10)</f>
         <v>7</v>
       </c>
@@ -708,19 +719,19 @@
       <c r="A11" s="2">
         <v>44691</v>
       </c>
-      <c r="B11" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="B11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E11" s="3">
         <v>4.5</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <f>SUM(B11:E11)</f>
         <v>5.5</v>
       </c>
@@ -729,19 +740,19 @@
       <c r="A12" s="2">
         <v>44692</v>
       </c>
-      <c r="B12" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0</v>
-      </c>
-      <c r="F12" s="4">
+      <c r="B12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3">
         <f>SUM(B12:E12)</f>
         <v>0.5</v>
       </c>
@@ -750,19 +761,19 @@
       <c r="A13" s="2">
         <v>44693</v>
       </c>
-      <c r="B13" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C13" s="4">
+      <c r="B13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C13" s="3">
         <v>10</v>
       </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0</v>
+      </c>
+      <c r="F13" s="3">
         <f>SUM(B13:E13)</f>
         <v>10.5</v>
       </c>
@@ -771,19 +782,19 @@
       <c r="A14" s="2">
         <v>44694</v>
       </c>
-      <c r="B14" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C14" s="4">
+      <c r="B14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C14" s="3">
         <v>1</v>
       </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0</v>
+      </c>
+      <c r="F14" s="3">
         <f>SUM(B14:E14)</f>
         <v>1.5</v>
       </c>
@@ -834,19 +845,19 @@
       <c r="A17" s="2">
         <v>44697</v>
       </c>
-      <c r="B17" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C17" s="4">
+      <c r="B17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C17" s="3">
         <v>1</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>1.5</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>6</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <f>SUM(B17:E17)</f>
         <v>9</v>
       </c>
@@ -855,19 +866,19 @@
       <c r="A18" s="2">
         <v>44698</v>
       </c>
-      <c r="B18" s="4">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
+      <c r="B18" s="3">
+        <v>0</v>
+      </c>
+      <c r="C18" s="3">
+        <v>0</v>
+      </c>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
         <v>7</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="3">
         <f>SUM(B18:E18)</f>
         <v>7</v>
       </c>
@@ -876,19 +887,19 @@
       <c r="A19" s="2">
         <v>44699</v>
       </c>
-      <c r="B19" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0</v>
-      </c>
-      <c r="F19" s="4">
+      <c r="B19" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C19" s="3">
+        <v>0</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3">
         <f>SUM(B19:E19)</f>
         <v>0.5</v>
       </c>
@@ -897,19 +908,19 @@
       <c r="A20" s="2">
         <v>44700</v>
       </c>
-      <c r="B20" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C20" s="4">
+      <c r="B20" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C20" s="3">
         <v>2.5</v>
       </c>
-      <c r="D20" s="4">
-        <v>0</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="D20" s="3">
+        <v>0</v>
+      </c>
+      <c r="E20" s="3">
         <v>6</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F20" s="3">
         <f>SUM(B20:E20)</f>
         <v>9</v>
       </c>
@@ -918,19 +929,19 @@
       <c r="A21" s="2">
         <v>44701</v>
       </c>
-      <c r="B21" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C21" s="4">
-        <v>0</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0</v>
-      </c>
-      <c r="F21" s="4">
+      <c r="B21" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C21" s="3">
+        <v>0</v>
+      </c>
+      <c r="D21" s="3">
+        <v>0</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0</v>
+      </c>
+      <c r="F21" s="3">
         <f>SUM(B21:E21)</f>
         <v>0.5</v>
       </c>
@@ -981,19 +992,19 @@
       <c r="A24" s="2">
         <v>44704</v>
       </c>
-      <c r="B24" s="4">
-        <v>0</v>
-      </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="4">
+      <c r="B24" s="3">
+        <v>0</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0</v>
+      </c>
+      <c r="D24" s="3">
+        <v>0</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0</v>
+      </c>
+      <c r="F24" s="3">
         <f>SUM(B24:E24)</f>
         <v>0</v>
       </c>
@@ -1002,19 +1013,19 @@
       <c r="A25" s="2">
         <v>44705</v>
       </c>
-      <c r="B25" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C25" s="4">
+      <c r="B25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C25" s="3">
         <v>7</v>
       </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="F25" s="4">
+      <c r="D25" s="3">
+        <v>0</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F25" s="3">
         <f>SUM(B25:E25)</f>
         <v>8</v>
       </c>
@@ -1023,19 +1034,19 @@
       <c r="A26" s="2">
         <v>44706</v>
       </c>
-      <c r="B26" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C26" s="4">
+      <c r="B26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C26" s="3">
         <v>9</v>
       </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="4">
+      <c r="D26" s="3">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0</v>
+      </c>
+      <c r="F26" s="3">
         <f>SUM(B26:E26)</f>
         <v>9.5</v>
       </c>
@@ -1044,19 +1055,19 @@
       <c r="A27" s="2">
         <v>44707</v>
       </c>
-      <c r="B27" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C27" s="4">
+      <c r="B27" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C27" s="3">
         <v>8.5</v>
       </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>0</v>
-      </c>
-      <c r="F27" s="4">
+      <c r="D27" s="3">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0</v>
+      </c>
+      <c r="F27" s="3">
         <f>SUM(B27:E27)</f>
         <v>9</v>
       </c>
@@ -1065,19 +1076,19 @@
       <c r="A28" s="2">
         <v>44708</v>
       </c>
-      <c r="B28" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="C28" s="4">
+      <c r="B28" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="C28" s="3">
         <v>7.5</v>
       </c>
-      <c r="D28" s="4">
-        <v>0</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="4">
+      <c r="D28" s="3">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0</v>
+      </c>
+      <c r="F28" s="3">
         <f>SUM(B28:E28)</f>
         <v>8</v>
       </c>
@@ -1128,19 +1139,19 @@
       <c r="A31" s="2">
         <v>44711</v>
       </c>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="F31" s="4">
+      <c r="B31" s="3">
+        <v>0</v>
+      </c>
+      <c r="C31" s="3">
+        <v>0</v>
+      </c>
+      <c r="D31" s="3">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
         <f>SUM(B31:E31)</f>
         <v>0</v>
       </c>
@@ -1167,23 +1178,23 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="4">
+      <c r="B33" s="3">
         <f>SUM(B2:B32)</f>
         <v>17.5</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="3">
         <f>SUM(C2:C32)</f>
         <v>57.5</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="3">
         <f>SUM(D2:D32)</f>
         <v>21</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E33" s="3">
         <f>SUM(E2:E32)</f>
         <v>31.5</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="12">
         <f>SUM(F2:F32)</f>
         <v>127.5</v>
       </c>
@@ -1194,12 +1205,12 @@
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="4" t="s">
+      <c r="A36" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="4" t="s">
+      <c r="A37" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1209,17 +1220,17 @@
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="4" t="s">
+      <c r="A40" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="4" t="s">
+      <c r="A41" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="4" t="s">
+      <c r="A42" s="4" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1229,7 +1240,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="4" t="s">
+      <c r="A45" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1239,37 +1250,37 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="4" t="s">
+      <c r="A48" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B49" s="4" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="4" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="4" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="4" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="4" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>